<commit_message>
END. buffer problem unsolved. if get som empty space input, buffer problem occurs.
</commit_message>
<xml_diff>
--- a/buildings.xlsx
+++ b/buildings.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Project\DB Basic\DB project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Project\DB Basic\Darnassus_Usher\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="buildings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,8 +23,173 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+  <si>
+    <t>달의 신전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피난처</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지팡이 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가죽 방어구 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬 방어구 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방패 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천 방어구 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양손무기 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투척 무기 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경매장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일용품점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가방 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>길드 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재봉용품 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가죽 세공용품 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다르나서스 여관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법 부여 용품점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 각인점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보석 세공점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>응급 치료원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광부 조합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기술 용품점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요리 용품점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연금술 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문 기술 교육, 상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세나리온 자치령 오른쪽 나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세나리온 자치령 가운데 나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자치령 건물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세나리온 자치령 왼쪽 나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다르나서스 입구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>울부짖는 참나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신전 정원 고목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,18 +513,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="C29" sqref="C29:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>